<commit_message>
Added new calc icon LineBuilder Further removed pandas for profiles and replaced them with numpy arrays
</commit_message>
<xml_diff>
--- a/Grids_and_profiles/grids/Some distribution grid.xlsx
+++ b/Grids_and_profiles/grids/Some distribution grid.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="182">
   <si>
     <t>Property</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Some distribution grid</t>
+  </si>
+  <si>
+    <t>nan</t>
   </si>
   <si>
     <t>GridCal</t>
@@ -145,7 +148,7 @@
     <t>66.0</t>
   </si>
   <si>
-    <t>10</t>
+    <t>10.0</t>
   </si>
   <si>
     <t>0.4</t>
@@ -160,64 +163,64 @@
     <t>0.0</t>
   </si>
   <si>
-    <t>-68.0</t>
+    <t>-461.0</t>
   </si>
   <si>
-    <t>-67.0</t>
+    <t>-460.0</t>
   </si>
   <si>
-    <t>22.124929062499987</t>
+    <t>-371.0</t>
   </si>
   <si>
-    <t>28.159000624999983</t>
+    <t>-365.0</t>
   </si>
   <si>
-    <t>46.261215312499985</t>
+    <t>-347.0</t>
   </si>
   <si>
-    <t>489.44365800624973</t>
+    <t>96.0</t>
   </si>
   <si>
-    <t>-526.683936332812</t>
+    <t>-919.0</t>
   </si>
   <si>
-    <t>-925.6869184031245</t>
+    <t>-1307.242411642412</t>
   </si>
   <si>
-    <t>909.7267991203121</t>
+    <t>542.8939708939707</t>
   </si>
   <si>
-    <t>518.703876691406</t>
+    <t>116.93180873180873</t>
+  </si>
+  <si>
+    <t>-550.0</t>
   </si>
   <si>
     <t>-355.0</t>
   </si>
   <si>
-    <t>-160.0</t>
+    <t>-83.0</t>
   </si>
   <si>
-    <t>112.63600249999993</t>
+    <t>205.0</t>
   </si>
   <si>
-    <t>400.2600803124998</t>
+    <t>494.0</t>
   </si>
   <si>
-    <t>689.8955153124998</t>
+    <t>-84.0</t>
   </si>
   <si>
-    <t>111.72083497968742</t>
+    <t>196.0</t>
   </si>
   <si>
-    <t>391.02292242890593</t>
+    <t>196.0149688149688</t>
   </si>
   <si>
-    <t>547.9640953765621</t>
+    <t>-77.22744282744281</t>
   </si>
   <si>
-    <t>263.3419681664061</t>
-  </si>
-  <si>
-    <t>723.5254074874997</t>
+    <t>501.10602910602915</t>
   </si>
   <si>
     <t>20.0</t>
@@ -322,19 +325,16 @@
     <t>1.0</t>
   </si>
   <si>
-    <t>7.890000000000001</t>
+    <t>7.8900000000000015</t>
   </si>
   <si>
-    <t>0.21600000000000003</t>
+    <t>0.21600000000000005</t>
   </si>
   <si>
-    <t>0</t>
+    <t>1.0000000000000001e-20</t>
   </si>
   <si>
-    <t>1e-20</t>
-  </si>
-  <si>
-    <t>1.898324</t>
+    <t>1.8983240000000001</t>
   </si>
   <si>
     <t>1.138995</t>
@@ -346,7 +346,7 @@
     <t>196.897853</t>
   </si>
   <si>
-    <t>131.265235</t>
+    <t>131.26523500000002</t>
   </si>
   <si>
     <t>0.05</t>
@@ -376,9 +376,6 @@
     <t>3e-06</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>5.0</t>
   </si>
   <si>
@@ -392,9 +389,6 @@
   </si>
   <si>
     <t>0.2</t>
-  </si>
-  <si>
-    <t>20</t>
   </si>
   <si>
     <t>0.0033</t>
@@ -446,9 +440,6 @@
   </si>
   <si>
     <t>Load@House 5</t>
-  </si>
-  <si>
-    <t>[ True]</t>
   </si>
   <si>
     <t>is_controlled</t>
@@ -571,25 +562,22 @@
     <t>B0</t>
   </si>
   <si>
-    <t>HV_nominal_voltage</t>
+    <t>HV</t>
   </si>
   <si>
-    <t>LV_nominal_voltage</t>
+    <t>LV</t>
   </si>
   <si>
-    <t>Nominal_power</t>
+    <t>Pcu</t>
   </si>
   <si>
-    <t>Copper_losses</t>
+    <t>Pfe</t>
   </si>
   <si>
-    <t>Iron_losses</t>
+    <t>I0</t>
   </si>
   <si>
-    <t>No_load_current</t>
-  </si>
-  <si>
-    <t>Short_circuit_voltage</t>
+    <t>Vsc</t>
   </si>
 </sst>
 </file>
@@ -1007,6 +995,9 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
@@ -1016,7 +1007,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1034,19 +1025,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -14504,25 +14495,25 @@
   <sheetData>
     <row r="1" spans="2:8">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -14540,73 +14531,73 @@
   <sheetData>
     <row r="1" spans="2:24">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="W1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -14624,52 +14615,52 @@
   <sheetData>
     <row r="1" spans="2:17">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="J1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -14687,25 +14678,25 @@
   <sheetData>
     <row r="1" spans="2:8">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -14723,28 +14714,28 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -14752,7 +14743,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C2">
         <v>1.050117</v>
@@ -14781,7 +14772,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C3">
         <v>0.379658</v>
@@ -14820,61 +14811,61 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="B1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -14882,7 +14873,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -14918,7 +14909,7 @@
         <v>0.54</v>
       </c>
       <c r="N2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -14944,7 +14935,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -14980,7 +14971,7 @@
         <v>0.54</v>
       </c>
       <c r="N3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="O3">
         <v>0.4</v>
@@ -15006,7 +14997,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -15042,7 +15033,7 @@
         <v>0.54</v>
       </c>
       <c r="N4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="O4">
         <v>0.8</v>
@@ -15068,7 +15059,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -15104,7 +15095,7 @@
         <v>0.789</v>
       </c>
       <c r="N5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -15130,7 +15121,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -15166,7 +15157,7 @@
         <v>0.789</v>
       </c>
       <c r="N6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O6">
         <v>0.5</v>
@@ -15192,7 +15183,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C7">
         <v>100</v>
@@ -15228,7 +15219,7 @@
         <v>0.789</v>
       </c>
       <c r="N7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -15256,18 +15247,18 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:J1"/>
+  <dimension ref="B1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:10">
+    <row r="1" spans="2:11">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>173</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>71</v>
@@ -15279,16 +15270,19 @@
         <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>172</v>
+        <v>74</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -15298,18 +15292,18 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:J1"/>
+  <dimension ref="B1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:10">
+    <row r="1" spans="2:11">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>173</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>71</v>
@@ -15321,16 +15315,19 @@
         <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>172</v>
+        <v>74</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -15348,28 +15345,28 @@
   <sheetData>
     <row r="1" spans="2:9">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -15387,49 +15384,49 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -15437,49 +15434,49 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -15487,49 +15484,49 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -15537,49 +15534,49 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -15587,49 +15584,49 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -15637,49 +15634,49 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -15687,49 +15684,49 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -15737,49 +15734,49 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -15787,49 +15784,49 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -15837,49 +15834,49 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -15887,49 +15884,49 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -15947,79 +15944,79 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:26">
@@ -16027,25 +16024,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G2" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s">
         <v>99</v>
@@ -16060,46 +16057,46 @@
         <v>99</v>
       </c>
       <c r="M2" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="N2" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="O2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P2" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="Q2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S2" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" t="s">
+        <v>63</v>
+      </c>
+      <c r="U2" t="s">
+        <v>119</v>
+      </c>
+      <c r="V2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X2" t="s">
         <v>120</v>
       </c>
-      <c r="T2" t="s">
-        <v>120</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="Y2" t="s">
         <v>121</v>
       </c>
-      <c r="V2" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" t="s">
-        <v>41</v>
-      </c>
-      <c r="X2" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>123</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -16107,25 +16104,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G3" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="H3" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s">
         <v>100</v>
@@ -16134,52 +16131,52 @@
         <v>106</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L3" t="s">
         <v>111</v>
       </c>
       <c r="M3" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="N3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P3" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="Q3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T3" t="s">
+        <v>63</v>
+      </c>
+      <c r="U3" t="s">
+        <v>119</v>
+      </c>
+      <c r="V3" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" t="s">
+        <v>42</v>
+      </c>
+      <c r="X3" t="s">
         <v>120</v>
       </c>
-      <c r="T3" t="s">
-        <v>120</v>
-      </c>
-      <c r="U3" t="s">
-        <v>121</v>
-      </c>
-      <c r="V3" t="s">
-        <v>41</v>
-      </c>
-      <c r="W3" t="s">
-        <v>41</v>
-      </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>122</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>124</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -16187,25 +16184,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G4" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="I4" t="s">
         <v>101</v>
@@ -16214,52 +16211,52 @@
         <v>107</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L4" t="s">
         <v>112</v>
       </c>
       <c r="M4" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="N4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P4" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="Q4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S4" t="s">
+        <v>63</v>
+      </c>
+      <c r="T4" t="s">
+        <v>63</v>
+      </c>
+      <c r="U4" t="s">
+        <v>119</v>
+      </c>
+      <c r="V4" t="s">
+        <v>42</v>
+      </c>
+      <c r="W4" t="s">
+        <v>42</v>
+      </c>
+      <c r="X4" t="s">
         <v>120</v>
       </c>
-      <c r="T4" t="s">
-        <v>120</v>
-      </c>
-      <c r="U4" t="s">
-        <v>121</v>
-      </c>
-      <c r="V4" t="s">
-        <v>41</v>
-      </c>
-      <c r="W4" t="s">
-        <v>41</v>
-      </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>122</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>124</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -16267,25 +16264,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G5" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="H5" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="I5" t="s">
         <v>102</v>
@@ -16294,52 +16291,52 @@
         <v>108</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L5" t="s">
         <v>113</v>
       </c>
       <c r="M5" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="N5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P5" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="Q5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T5" t="s">
+        <v>63</v>
+      </c>
+      <c r="U5" t="s">
+        <v>119</v>
+      </c>
+      <c r="V5" t="s">
+        <v>42</v>
+      </c>
+      <c r="W5" t="s">
+        <v>42</v>
+      </c>
+      <c r="X5" t="s">
         <v>120</v>
       </c>
-      <c r="T5" t="s">
-        <v>120</v>
-      </c>
-      <c r="U5" t="s">
-        <v>121</v>
-      </c>
-      <c r="V5" t="s">
-        <v>41</v>
-      </c>
-      <c r="W5" t="s">
-        <v>41</v>
-      </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>122</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>124</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -16347,25 +16344,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G6" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="I6" t="s">
         <v>99</v>
@@ -16380,46 +16377,46 @@
         <v>99</v>
       </c>
       <c r="M6" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="N6" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="O6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P6" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="Q6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S6" t="s">
+        <v>63</v>
+      </c>
+      <c r="T6" t="s">
+        <v>63</v>
+      </c>
+      <c r="U6" t="s">
+        <v>119</v>
+      </c>
+      <c r="V6" t="s">
+        <v>42</v>
+      </c>
+      <c r="W6" t="s">
+        <v>42</v>
+      </c>
+      <c r="X6" t="s">
         <v>120</v>
       </c>
-      <c r="T6" t="s">
-        <v>120</v>
-      </c>
-      <c r="U6" t="s">
+      <c r="Y6" t="s">
         <v>121</v>
       </c>
-      <c r="V6" t="s">
-        <v>41</v>
-      </c>
-      <c r="W6" t="s">
-        <v>41</v>
-      </c>
-      <c r="X6" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>123</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -16427,25 +16424,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G7" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="H7" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="I7" t="s">
         <v>99</v>
@@ -16460,46 +16457,46 @@
         <v>99</v>
       </c>
       <c r="M7" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="N7" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="O7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P7" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="Q7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U7" t="s">
+        <v>119</v>
+      </c>
+      <c r="V7" t="s">
+        <v>42</v>
+      </c>
+      <c r="W7" t="s">
+        <v>42</v>
+      </c>
+      <c r="X7" t="s">
         <v>120</v>
       </c>
-      <c r="T7" t="s">
-        <v>120</v>
-      </c>
-      <c r="U7" t="s">
+      <c r="Y7" t="s">
         <v>121</v>
       </c>
-      <c r="V7" t="s">
-        <v>41</v>
-      </c>
-      <c r="W7" t="s">
-        <v>41</v>
-      </c>
-      <c r="X7" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>123</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -16507,25 +16504,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G8" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="H8" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="I8" t="s">
         <v>103</v>
@@ -16534,52 +16531,52 @@
         <v>109</v>
       </c>
       <c r="K8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M8" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="N8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P8" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="Q8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T8" t="s">
+        <v>63</v>
+      </c>
+      <c r="U8" t="s">
+        <v>119</v>
+      </c>
+      <c r="V8" t="s">
+        <v>42</v>
+      </c>
+      <c r="W8" t="s">
+        <v>42</v>
+      </c>
+      <c r="X8" t="s">
         <v>120</v>
       </c>
-      <c r="T8" t="s">
-        <v>120</v>
-      </c>
-      <c r="U8" t="s">
-        <v>121</v>
-      </c>
-      <c r="V8" t="s">
-        <v>41</v>
-      </c>
-      <c r="W8" t="s">
-        <v>41</v>
-      </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>122</v>
       </c>
-      <c r="Y8" t="s">
-        <v>124</v>
-      </c>
       <c r="Z8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -16587,25 +16584,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G9" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="H9" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="I9" t="s">
         <v>104</v>
@@ -16614,52 +16611,52 @@
         <v>110</v>
       </c>
       <c r="K9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M9" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="N9" t="s">
+        <v>118</v>
+      </c>
+      <c r="O9" t="s">
+        <v>96</v>
+      </c>
+      <c r="P9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>36</v>
+      </c>
+      <c r="R9" t="s">
+        <v>96</v>
+      </c>
+      <c r="S9" t="s">
+        <v>63</v>
+      </c>
+      <c r="T9" t="s">
+        <v>63</v>
+      </c>
+      <c r="U9" t="s">
         <v>119</v>
       </c>
-      <c r="O9" t="s">
-        <v>95</v>
-      </c>
-      <c r="P9" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>35</v>
-      </c>
-      <c r="R9" t="s">
-        <v>95</v>
-      </c>
-      <c r="S9" t="s">
+      <c r="V9" t="s">
+        <v>42</v>
+      </c>
+      <c r="W9" t="s">
+        <v>42</v>
+      </c>
+      <c r="X9" t="s">
         <v>120</v>
       </c>
-      <c r="T9" t="s">
-        <v>120</v>
-      </c>
-      <c r="U9" t="s">
-        <v>121</v>
-      </c>
-      <c r="V9" t="s">
-        <v>41</v>
-      </c>
-      <c r="W9" t="s">
-        <v>41</v>
-      </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>122</v>
       </c>
-      <c r="Y9" t="s">
-        <v>124</v>
-      </c>
       <c r="Z9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -16667,25 +16664,25 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G10" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="H10" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="I10" t="s">
         <v>99</v>
@@ -16700,46 +16697,46 @@
         <v>99</v>
       </c>
       <c r="M10" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="N10" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="O10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P10" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="Q10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S10" t="s">
+        <v>63</v>
+      </c>
+      <c r="T10" t="s">
+        <v>63</v>
+      </c>
+      <c r="U10" t="s">
+        <v>119</v>
+      </c>
+      <c r="V10" t="s">
+        <v>42</v>
+      </c>
+      <c r="W10" t="s">
+        <v>42</v>
+      </c>
+      <c r="X10" t="s">
         <v>120</v>
       </c>
-      <c r="T10" t="s">
-        <v>120</v>
-      </c>
-      <c r="U10" t="s">
+      <c r="Y10" t="s">
         <v>121</v>
       </c>
-      <c r="V10" t="s">
-        <v>41</v>
-      </c>
-      <c r="W10" t="s">
-        <v>41</v>
-      </c>
-      <c r="X10" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y10" t="s">
+      <c r="Z10" t="s">
         <v>123</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -16757,37 +16754,37 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -16795,13 +16792,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s">
-        <v>138</v>
+        <v>30</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0.0110354300759503</v>
@@ -16833,13 +16830,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>138</v>
+        <v>31</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0.0108575434295839</v>
@@ -16871,13 +16868,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>138</v>
+        <v>32</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
       </c>
       <c r="E4">
         <v>0.0206397483581723</v>
@@ -16909,13 +16906,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>138</v>
+        <v>33</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
       </c>
       <c r="E5">
         <v>0.0138164486929629</v>
@@ -16947,13 +16944,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>138</v>
+        <v>34</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
       </c>
       <c r="E6">
         <v>0.0111468755031423</v>
@@ -16995,19 +16992,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -30465,19 +30462,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -43935,19 +43932,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -57405,19 +57402,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -70875,19 +70872,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>